<commit_message>
Thesis continuing and tests for pictures
</commit_message>
<xml_diff>
--- a/bicriteriaTableSafe.xlsx
+++ b/bicriteriaTableSafe.xlsx
@@ -391,14 +391,14 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N26" activeCellId="0" sqref="N26"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="3" min="3" style="0" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.71"/>
@@ -425,7 +425,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>

</xml_diff>